<commit_message>
REPORTGEN-703: fix issue and update CISQ excel reports
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/CISQ Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/CISQ Full Detailed Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52276090-7BD2-4A91-A10C-D2CAE8DFB072}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7E670F-0276-42E2-84CE-F5024D654B78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>Application Name:</t>
   </si>
@@ -77,70 +77,106 @@
     <t>RepGen:TEXT;METRIC_TECHNICAL_DEBT</t>
   </si>
   <si>
-    <t>RepGen:TABLE;TECHNICAL_SIZING</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=CISQ,LBL=violations,MORE=true</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=CISQ-Security,COUNT=-1</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=CISQ-Security,LBL=violations</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=CISQ-Reliability,LBL=violations</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=CISQ-Reliability,COUNT=-1</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=CISQ-Performance-Efficiency,LBL=violations</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=CISQ-Performance-Efficiency,COUNT=-1</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=CISQ-Maintainability,LBL=violations</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=CISQ-Maintainability,COUNT=-1</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;TECHNO_LOC</t>
-  </si>
-  <si>
     <t>CISQ Compliance details</t>
   </si>
   <si>
     <t>Application characteristics</t>
   </si>
   <si>
-    <t>Findings summary for CAST under CISQ Standards</t>
-  </si>
-  <si>
-    <t>CAST findings for CISQ Security</t>
-  </si>
-  <si>
-    <t>CAST findings detail for CISQ Maintainability</t>
-  </si>
-  <si>
-    <t>CAST findings for CISQ Maintainability</t>
-  </si>
-  <si>
-    <t>CAST findings details for CISQ Performance Efficiency</t>
-  </si>
-  <si>
-    <t>CAST findings for CISQ Performance Efficiency</t>
-  </si>
-  <si>
-    <t>CAST findings details for CISQ Reliability</t>
-  </si>
-  <si>
-    <t>CAST findings for CISQ Reliability</t>
-  </si>
-  <si>
-    <t>CAST findings details for CISQ Security</t>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Lines of Code</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;TECHNO_LOC;HEADER=NO</t>
+  </si>
+  <si>
+    <t>Characteristic</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;TECHNICAL_SIZING;HEADER=NO</t>
+  </si>
+  <si>
+    <t>Findings summary for CAST under CISQ Security Standards</t>
+  </si>
+  <si>
+    <t>Quality Standard</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=CISQ,MORE=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>Rules</t>
+  </si>
+  <si>
+    <t>Rationale</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Remediation</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=CISQ-Security,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>Rule Name</t>
+  </si>
+  <si>
+    <t>Object Name</t>
+  </si>
+  <si>
+    <t>Object Type</t>
+  </si>
+  <si>
+    <t>Violation Status</t>
+  </si>
+  <si>
+    <t>Associated Value</t>
+  </si>
+  <si>
+    <t>File Path</t>
+  </si>
+  <si>
+    <t>Start Line</t>
+  </si>
+  <si>
+    <t>End Line</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=CISQ-Security,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=CISQ-Reliability,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=CISQ-Reliability,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=CISQ-Performance-Efficiency,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=CISQ-Performance-Efficiency,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=CISQ-Maintainability,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=CISQ-Maintainability,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>Total Violations</t>
+  </si>
+  <si>
+    <t>Added Violations</t>
+  </si>
+  <si>
+    <t>Removed Violations</t>
   </si>
 </sst>
 </file>
@@ -347,7 +383,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -396,27 +432,37 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -794,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O13"/>
+  <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -823,12 +869,12 @@
       <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="2"/>
@@ -837,10 +883,10 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
@@ -853,10 +899,10 @@
       </c>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
@@ -872,29 +918,64 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
+      <c r="B6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>10</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D9" s="21"/>
       <c r="N9" s="17"/>
       <c r="O9" s="16"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
+      <c r="B12" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -910,28 +991,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="88.21875" customWidth="1"/>
     <col min="2" max="2" width="24.5546875" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.88671875" customWidth="1"/>
+    <col min="6" max="6" width="42.21875" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -941,7 +1050,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00038B0F-4F74-4ACF-8A7F-FE15A067CF76}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -949,18 +1058,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="G1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -971,29 +1107,56 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199C8C5D-EC74-404D-8E71-79059E3D9694}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="103.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="88.21875" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.88671875" customWidth="1"/>
+    <col min="6" max="6" width="42.21875" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1003,7 +1166,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B659E30C-CCFD-4222-A0CA-F3DF515BD633}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1011,18 +1174,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="E1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1033,26 +1223,56 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD2417C-E545-422E-BF8A-D513D7E3FCC6}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="103.77734375" customWidth="1"/>
-    <col min="2" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="93.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.88671875" customWidth="1"/>
+    <col min="6" max="6" width="42.21875" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1062,26 +1282,53 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB238E2-139C-4ACF-A6AA-64C78522FF51}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="105.44140625" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1092,29 +1339,56 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83EA1EA1-1BE2-491B-B922-C115919AD451}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="103.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="88.21875" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.88671875" customWidth="1"/>
+    <col min="6" max="6" width="42.21875" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1124,26 +1398,53 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A03D1F2-D140-4212-A036-86834BE44347}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="97.5546875" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-709: update full detailed excel reports
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/CISQ Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/CISQ Full Detailed Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7E670F-0276-42E2-84CE-F5024D654B78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03359EA-870B-4483-9370-8789301D85D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -449,20 +449,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -843,7 +837,7 @@
   <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,8 +863,8 @@
       <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
@@ -883,13 +877,13 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
+      <c r="D3" s="11"/>
       <c r="E3" s="12"/>
       <c r="F3" s="9" t="s">
         <v>4</v>
@@ -899,13 +893,13 @@
       </c>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="13"/>
       <c r="F4" s="7" t="s">
         <v>2</v>
@@ -978,10 +972,8 @@
       <c r="E14" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>